<commit_message>
Update test files after adjust-to-content has been refactored.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Comments/AddingComments.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Comments/AddingComments.xlsx
@@ -803,7 +803,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
     <x:t>Hidden</x:t>
   </x:si>
@@ -1288,7 +1288,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="23.580625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="23.853482" style="0" customWidth="1"/>
     <x:col min="2" max="4" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>

</xml_diff>

<commit_message>
#1969 Replace the dictionary XLCell storage in XLCellsCollection with a sparse arrays, separated to several slices (values, formulas, styles, misc). The key benefit at this time is decreased memory consumption, but in longer term, it will allow better bulk operations and speedup of range insert/delete due to better structure.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Comments/AddingComments.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Comments/AddingComments.xlsx
@@ -1181,8 +1181,6 @@
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="E1" s="0"/>
-      <x:c r="G1" s="0"/>
     </x:row>
     <x:row r="2" spans="1:11">
       <x:c r="A2" s="0" t="s">
@@ -1193,23 +1191,14 @@
       <x:c r="A3" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="E3" s="0"/>
-      <x:c r="G3" s="0"/>
     </x:row>
     <x:row r="4" spans="1:11">
       <x:c r="A4" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:11">
-      <x:c r="E7" s="0"/>
-    </x:row>
-    <x:row r="9" spans="1:11">
-      <x:c r="A9" s="0"/>
-      <x:c r="D9" s="0"/>
-      <x:c r="E9" s="0"/>
-      <x:c r="F9" s="0"/>
-    </x:row>
+    <x:row r="7" spans="1:11"/>
+    <x:row r="9" spans="1:11"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1234,12 +1223,8 @@
     <x:col min="1" max="5" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="2" spans="1:5">
-      <x:c r="A2" s="0"/>
-    </x:row>
-    <x:row r="4" spans="1:5">
-      <x:c r="A4" s="0"/>
-    </x:row>
+    <x:row r="2" spans="1:5"/>
+    <x:row r="4" spans="1:5"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1264,9 +1249,7 @@
     <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4">
-      <x:c r="A1" s="0"/>
-    </x:row>
+    <x:row r="1" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1297,15 +1280,9 @@
         <x:v>4</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:4">
-      <x:c r="A2" s="0"/>
-    </x:row>
-    <x:row r="3" spans="1:4">
-      <x:c r="A3" s="0"/>
-    </x:row>
-    <x:row r="4" spans="1:4">
-      <x:c r="A4" s="0"/>
-    </x:row>
+    <x:row r="2" spans="1:4"/>
+    <x:row r="3" spans="1:4"/>
+    <x:row r="4" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1330,9 +1307,7 @@
     <x:col min="1" max="5" width="10.710625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5">
-      <x:c r="A1" s="0"/>
-    </x:row>
+    <x:row r="1" spans="1:5"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1357,9 +1332,7 @@
     <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="2" spans="1:4">
-      <x:c r="A2" s="0"/>
-    </x:row>
+    <x:row r="2" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1384,18 +1357,9 @@
     <x:col min="1" max="9" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:9">
-      <x:c r="A1" s="0"/>
-    </x:row>
-    <x:row r="3" spans="1:9">
-      <x:c r="A3" s="0"/>
-      <x:c r="D3" s="0"/>
-      <x:c r="E3" s="0"/>
-      <x:c r="F3" s="0"/>
-    </x:row>
-    <x:row r="8" spans="1:9">
-      <x:c r="A8" s="0"/>
-    </x:row>
+    <x:row r="1" spans="1:9"/>
+    <x:row r="3" spans="1:9"/>
+    <x:row r="8" spans="1:9"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1420,9 +1384,7 @@
     <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="2" spans="1:4">
-      <x:c r="A2" s="0"/>
-    </x:row>
+    <x:row r="2" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1447,9 +1409,7 @@
     <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="2" spans="1:4">
-      <x:c r="A2" s="0"/>
-    </x:row>
+    <x:row r="2" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1474,15 +1434,9 @@
     <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4">
-      <x:c r="A1" s="0"/>
-    </x:row>
-    <x:row r="2" spans="1:4">
-      <x:c r="A2" s="0"/>
-    </x:row>
-    <x:row r="3" spans="1:4">
-      <x:c r="A3" s="0"/>
-    </x:row>
+    <x:row r="1" spans="1:4"/>
+    <x:row r="2" spans="1:4"/>
+    <x:row r="3" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1507,9 +1461,7 @@
     <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4">
-      <x:c r="A1" s="0"/>
-    </x:row>
+    <x:row r="1" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>